<commit_message>
Style: Ajout des Ice rule tiles and intégration pour le biome de glace
</commit_message>
<xml_diff>
--- a/C61/Sprint 1/C61 - Sprint1c - Outil de planification.xlsx
+++ b/C61/Sprint 1/C61 - Sprint1c - Outil de planification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1370770\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur.UTILISA-7INSOVG\Desktop\GeeksLegacy\C61\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2928058F-BD06-49EC-B320-ABA4582A3B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAF4AFD-599D-4FCA-BE1F-DD35415D84FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,17 +45,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -817,9 +806,6 @@
     <t>AF</t>
   </si>
   <si>
-    <t>Convevoir les objets (matériels) et les programmer</t>
-  </si>
-  <si>
     <t>Programmer le mécaniques d'attaque des ennemis.</t>
   </si>
   <si>
@@ -830,6 +816,9 @@
   </si>
   <si>
     <t>Déployer le jeu</t>
+  </si>
+  <si>
+    <t>Concevoir les objets (matériels) et les programmer</t>
   </si>
 </sst>
 </file>
@@ -1206,11 +1195,26 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1226,21 +1230,6 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -7488,8 +7477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AF97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="M34" sqref="D34:M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -7511,54 +7500,54 @@
     <row r="1" spans="2:31" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:31" ht="25.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="17"/>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
     </row>
     <row r="3" spans="2:31" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
     </row>
     <row r="4" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:31" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="18"/>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="2:31" ht="6.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I6" s="15"/>
@@ -7579,12 +7568,12 @@
         <v>5</v>
       </c>
       <c r="I7" s="15"/>
-      <c r="J7" s="45" t="s">
+      <c r="J7" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
       <c r="N7" s="38">
         <v>2</v>
       </c>
@@ -7647,20 +7636,20 @@
     <row r="12" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="2:31" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="18"/>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
       <c r="U13" s="2">
         <f>D68</f>
         <v>36</v>
@@ -7675,12 +7664,12 @@
       <c r="C15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
       <c r="H15" s="5" t="s">
         <v>14</v>
       </c>
@@ -7731,12 +7720,12 @@
       <c r="C16" s="11">
         <v>1</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="30"/>
       <c r="I16" s="30" t="s">
         <v>25</v>
@@ -7757,7 +7746,7 @@
         <v>27</v>
       </c>
       <c r="T16" s="1" t="b">
-        <f t="shared" ref="T16:T28" si="1">ISBLANK(D16)</f>
+        <f t="shared" ref="T16:T27" si="1">ISBLANK(D16)</f>
         <v>0</v>
       </c>
       <c r="AA16" s="1"/>
@@ -7775,12 +7764,12 @@
       <c r="C17" s="12">
         <v>2</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
       <c r="H17" s="32">
         <v>1</v>
       </c>
@@ -7844,12 +7833,12 @@
       <c r="C18" s="13">
         <v>3</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
       <c r="H18" s="34">
         <v>2</v>
       </c>
@@ -7917,12 +7906,12 @@
       <c r="C19" s="12">
         <v>4</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D19" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
       <c r="H19" s="32">
         <v>3</v>
       </c>
@@ -7990,12 +7979,12 @@
       <c r="C20" s="13">
         <v>5</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
       <c r="H20" s="34">
         <v>3</v>
       </c>
@@ -8051,12 +8040,12 @@
       <c r="C21" s="12">
         <v>6</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
       <c r="H21" s="32">
         <v>5</v>
       </c>
@@ -8097,12 +8086,12 @@
       <c r="C22" s="13">
         <v>7</v>
       </c>
-      <c r="D22" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
+      <c r="D22" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
       <c r="H22" s="34">
         <v>3</v>
       </c>
@@ -8139,12 +8128,12 @@
       <c r="C23" s="12">
         <v>8</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
       <c r="H23" s="32">
         <v>3</v>
       </c>
@@ -8190,12 +8179,12 @@
       <c r="C24" s="13">
         <v>9</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
       <c r="H24" s="34">
         <v>8</v>
       </c>
@@ -8244,12 +8233,12 @@
       <c r="C25" s="12">
         <v>10</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="D25" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
       <c r="H25" s="32">
         <v>3</v>
       </c>
@@ -8298,12 +8287,12 @@
       <c r="C26" s="13">
         <v>11</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
       <c r="H26" s="34">
         <v>6</v>
       </c>
@@ -8352,12 +8341,12 @@
       <c r="C27" s="12">
         <v>12</v>
       </c>
-      <c r="D27" s="39" t="s">
+      <c r="D27" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
       <c r="H27" s="32">
         <v>11</v>
       </c>
@@ -8406,12 +8395,12 @@
       <c r="C28" s="13">
         <v>13</v>
       </c>
-      <c r="D28" s="40" t="s">
-        <v>102</v>
-      </c>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
+      <c r="D28" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
       <c r="H28" s="34">
         <v>3</v>
       </c>
@@ -8434,7 +8423,7 @@
         <v>27</v>
       </c>
       <c r="T28" s="1" t="b">
-        <f>ISBLANK(D29)</f>
+        <f t="shared" ref="T28:T36" si="4">ISBLANK(D29)</f>
         <v>0</v>
       </c>
       <c r="U28" s="2">
@@ -8460,12 +8449,12 @@
       <c r="C29" s="12">
         <v>14</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
       <c r="H29" s="32">
         <v>12</v>
       </c>
@@ -8488,7 +8477,7 @@
         <v>100</v>
       </c>
       <c r="T29" s="1" t="b">
-        <f>ISBLANK(D30)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U29" s="2">
@@ -8502,12 +8491,12 @@
       <c r="C30" s="13">
         <v>15</v>
       </c>
-      <c r="D30" s="39" t="s">
+      <c r="D30" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
       <c r="H30" s="34">
         <v>3</v>
       </c>
@@ -8530,7 +8519,7 @@
         <v>100</v>
       </c>
       <c r="T30" s="1" t="b">
-        <f>ISBLANK(D31)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U30" s="2">
@@ -8550,12 +8539,12 @@
       <c r="C31" s="12">
         <v>16</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
       <c r="H31" s="32">
         <v>3</v>
       </c>
@@ -8578,7 +8567,7 @@
         <v>101</v>
       </c>
       <c r="T31" s="1" t="b">
-        <f>ISBLANK(D32)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U31" s="2">
@@ -8603,12 +8592,12 @@
       <c r="C32" s="13">
         <v>17</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="D32" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
       <c r="H32" s="34">
         <v>16</v>
       </c>
@@ -8631,7 +8620,7 @@
         <v>101</v>
       </c>
       <c r="T32" s="1" t="b">
-        <f>ISBLANK(D33)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U32" s="2">
@@ -8656,12 +8645,12 @@
       <c r="C33" s="12">
         <v>18</v>
       </c>
-      <c r="D33" s="40" t="s">
+      <c r="D33" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
       <c r="H33" s="32">
         <v>16</v>
       </c>
@@ -8684,7 +8673,7 @@
         <v>100</v>
       </c>
       <c r="T33" s="1" t="b">
-        <f>ISBLANK(D34)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U33" s="2">
@@ -8709,12 +8698,12 @@
       <c r="C34" s="13">
         <v>19</v>
       </c>
-      <c r="D34" s="39" t="s">
+      <c r="D34" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
       <c r="H34" s="34">
         <v>17</v>
       </c>
@@ -8737,7 +8726,7 @@
         <v>27</v>
       </c>
       <c r="T34" s="1" t="b">
-        <f>ISBLANK(D35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U34" s="2">
@@ -8751,12 +8740,12 @@
       <c r="C35" s="12">
         <v>20</v>
       </c>
-      <c r="D35" s="47" t="s">
+      <c r="D35" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
       <c r="H35" s="32">
         <v>16</v>
       </c>
@@ -8779,7 +8768,7 @@
         <v>100</v>
       </c>
       <c r="T35" s="1" t="b">
-        <f>ISBLANK(D36)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U35" s="2">
@@ -8799,12 +8788,12 @@
       <c r="C36" s="13">
         <v>21</v>
       </c>
-      <c r="D36" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
+      <c r="D36" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
       <c r="H36" s="34">
         <v>17</v>
       </c>
@@ -8827,7 +8816,7 @@
         <v>100</v>
       </c>
       <c r="T36" s="1" t="b">
-        <f>ISBLANK(D37)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U36" s="2">
@@ -8852,12 +8841,12 @@
       <c r="C37" s="12">
         <v>22</v>
       </c>
-      <c r="D37" s="40" t="s">
+      <c r="D37" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
       <c r="H37" s="32">
         <v>3</v>
       </c>
@@ -8905,12 +8894,12 @@
       <c r="C38" s="13">
         <v>23</v>
       </c>
-      <c r="D38" s="40" t="s">
+      <c r="D38" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
       <c r="H38" s="34">
         <v>22</v>
       </c>
@@ -8958,12 +8947,12 @@
       <c r="C39" s="12">
         <v>24</v>
       </c>
-      <c r="D39" s="39" t="s">
+      <c r="D39" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
       <c r="H39" s="32">
         <v>23</v>
       </c>
@@ -9000,12 +8989,12 @@
       <c r="C40" s="13">
         <v>25</v>
       </c>
-      <c r="D40" s="40" t="s">
+      <c r="D40" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="E40" s="40"/>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
       <c r="H40" s="34">
         <v>19</v>
       </c>
@@ -9048,12 +9037,12 @@
       <c r="C41" s="12">
         <v>26</v>
       </c>
-      <c r="D41" s="39" t="s">
+      <c r="D41" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="40"/>
       <c r="H41" s="32">
         <v>12</v>
       </c>
@@ -9101,12 +9090,12 @@
       <c r="C42" s="13">
         <v>27</v>
       </c>
-      <c r="D42" s="40" t="s">
+      <c r="D42" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
       <c r="H42" s="34">
         <v>20</v>
       </c>
@@ -9154,12 +9143,12 @@
       <c r="C43" s="12">
         <v>28</v>
       </c>
-      <c r="D43" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
+      <c r="D43" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="40"/>
       <c r="H43" s="32">
         <v>10</v>
       </c>
@@ -9207,12 +9196,12 @@
       <c r="C44" s="13">
         <v>29</v>
       </c>
-      <c r="D44" s="40" t="s">
+      <c r="D44" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
       <c r="H44" s="34">
         <v>27</v>
       </c>
@@ -9235,7 +9224,7 @@
         <v>27</v>
       </c>
       <c r="T44" s="1" t="b">
-        <f t="shared" ref="T44:T50" si="4">ISBLANK(D44)</f>
+        <f t="shared" ref="T44:T50" si="5">ISBLANK(D44)</f>
         <v>0</v>
       </c>
       <c r="U44" s="2">
@@ -9249,12 +9238,12 @@
       <c r="C45" s="12">
         <v>30</v>
       </c>
-      <c r="D45" s="39" t="s">
+      <c r="D45" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
       <c r="H45" s="32">
         <v>6</v>
       </c>
@@ -9277,7 +9266,7 @@
         <v>27</v>
       </c>
       <c r="T45" s="1" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U45" s="2">
@@ -9291,12 +9280,12 @@
       <c r="C46" s="13">
         <v>31</v>
       </c>
-      <c r="D46" s="40" t="s">
+      <c r="D46" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="39"/>
       <c r="H46" s="34">
         <v>27</v>
       </c>
@@ -9319,7 +9308,7 @@
         <v>27</v>
       </c>
       <c r="T46" s="1" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U46" s="2">
@@ -9333,12 +9322,12 @@
       <c r="C47" s="12">
         <v>32</v>
       </c>
-      <c r="D47" s="39" t="s">
+      <c r="D47" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
       <c r="H47" s="32">
         <v>7</v>
       </c>
@@ -9361,7 +9350,7 @@
         <v>27</v>
       </c>
       <c r="T47" s="1" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U47" s="2">
@@ -9375,12 +9364,12 @@
       <c r="C48" s="13">
         <v>33</v>
       </c>
-      <c r="D48" s="40" t="s">
+      <c r="D48" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
       <c r="H48" s="34">
         <v>19</v>
       </c>
@@ -9403,7 +9392,7 @@
         <v>27</v>
       </c>
       <c r="T48" s="1" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U48" s="2">
@@ -9417,12 +9406,12 @@
       <c r="C49" s="12">
         <v>34</v>
       </c>
-      <c r="D49" s="39" t="s">
+      <c r="D49" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="39"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="40"/>
       <c r="H49" s="32">
         <v>10</v>
       </c>
@@ -9445,7 +9434,7 @@
         <v>27</v>
       </c>
       <c r="T49" s="1" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U49" s="2">
@@ -9462,12 +9451,12 @@
       <c r="C50" s="13">
         <v>35</v>
       </c>
-      <c r="D50" s="40" t="s">
+      <c r="D50" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="E50" s="40"/>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
       <c r="H50" s="34">
         <v>19</v>
       </c>
@@ -9490,7 +9479,7 @@
         <v>27</v>
       </c>
       <c r="T50" s="1" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U50" s="2">
@@ -9507,12 +9496,12 @@
       <c r="C51" s="12">
         <v>36</v>
       </c>
-      <c r="D51" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="E51" s="39"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="39"/>
+      <c r="D51" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
       <c r="H51" s="32">
         <v>5</v>
       </c>
@@ -9535,7 +9524,7 @@
         <v>27</v>
       </c>
       <c r="T51" s="1" t="b">
-        <f t="shared" ref="T51:T65" si="5">ISBLANK(D51)</f>
+        <f t="shared" ref="T51:T65" si="6">ISBLANK(D51)</f>
         <v>0</v>
       </c>
       <c r="U51" s="2">
@@ -9552,10 +9541,10 @@
       <c r="C52" s="13">
         <v>37</v>
       </c>
-      <c r="D52" s="40"/>
-      <c r="E52" s="40"/>
-      <c r="F52" s="40"/>
-      <c r="G52" s="40"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="39"/>
       <c r="H52" s="34"/>
       <c r="I52" s="34"/>
       <c r="J52" s="34"/>
@@ -9564,7 +9553,7 @@
       <c r="M52" s="34"/>
       <c r="N52" s="34"/>
       <c r="T52" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U52" s="2">
@@ -9581,10 +9570,10 @@
       <c r="C53" s="12">
         <v>38</v>
       </c>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="40"/>
       <c r="H53" s="32"/>
       <c r="I53" s="32"/>
       <c r="J53" s="32"/>
@@ -9593,7 +9582,7 @@
       <c r="M53" s="32"/>
       <c r="N53" s="32"/>
       <c r="T53" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U53" s="2">
@@ -9610,10 +9599,10 @@
       <c r="C54" s="13">
         <v>39</v>
       </c>
-      <c r="D54" s="40"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="40"/>
-      <c r="G54" s="40"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
       <c r="H54" s="34"/>
       <c r="I54" s="34"/>
       <c r="J54" s="34"/>
@@ -9622,7 +9611,7 @@
       <c r="M54" s="34"/>
       <c r="N54" s="34"/>
       <c r="T54" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U54" s="2">
@@ -9639,10 +9628,10 @@
       <c r="C55" s="12">
         <v>40</v>
       </c>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="39"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
       <c r="H55" s="32"/>
       <c r="I55" s="32"/>
       <c r="J55" s="32"/>
@@ -9651,7 +9640,7 @@
       <c r="M55" s="32"/>
       <c r="N55" s="32"/>
       <c r="T55" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U55" s="2">
@@ -9668,10 +9657,10 @@
       <c r="C56" s="13">
         <v>41</v>
       </c>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
       <c r="H56" s="34"/>
       <c r="I56" s="34"/>
       <c r="J56" s="34"/>
@@ -9680,7 +9669,7 @@
       <c r="M56" s="34"/>
       <c r="N56" s="34"/>
       <c r="T56" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U56" s="2">
@@ -9697,10 +9686,10 @@
       <c r="C57" s="12">
         <v>42</v>
       </c>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="39"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="40"/>
       <c r="H57" s="32"/>
       <c r="I57" s="32"/>
       <c r="J57" s="32"/>
@@ -9709,7 +9698,7 @@
       <c r="M57" s="32"/>
       <c r="N57" s="32"/>
       <c r="T57" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U57" s="2">
@@ -9726,10 +9715,10 @@
       <c r="C58" s="13">
         <v>43</v>
       </c>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="39"/>
       <c r="H58" s="34"/>
       <c r="I58" s="34"/>
       <c r="J58" s="34"/>
@@ -9738,7 +9727,7 @@
       <c r="M58" s="34"/>
       <c r="N58" s="34"/>
       <c r="T58" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U58" s="2">
@@ -9755,10 +9744,10 @@
       <c r="C59" s="12">
         <v>44</v>
       </c>
-      <c r="D59" s="39"/>
-      <c r="E59" s="39"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="40"/>
       <c r="H59" s="32"/>
       <c r="I59" s="32"/>
       <c r="J59" s="32"/>
@@ -9767,7 +9756,7 @@
       <c r="M59" s="32"/>
       <c r="N59" s="32"/>
       <c r="T59" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U59" s="2">
@@ -9784,10 +9773,10 @@
       <c r="C60" s="13">
         <v>45</v>
       </c>
-      <c r="D60" s="40"/>
-      <c r="E60" s="40"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="40"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39"/>
       <c r="H60" s="34"/>
       <c r="I60" s="34"/>
       <c r="J60" s="34"/>
@@ -9796,7 +9785,7 @@
       <c r="M60" s="34"/>
       <c r="N60" s="34"/>
       <c r="T60" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U60" s="2">
@@ -9813,10 +9802,10 @@
       <c r="C61" s="12">
         <v>46</v>
       </c>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="40"/>
       <c r="H61" s="32"/>
       <c r="I61" s="32"/>
       <c r="J61" s="32"/>
@@ -9825,7 +9814,7 @@
       <c r="M61" s="32"/>
       <c r="N61" s="32"/>
       <c r="T61" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U61" s="2">
@@ -9842,10 +9831,10 @@
       <c r="C62" s="13">
         <v>47</v>
       </c>
-      <c r="D62" s="40"/>
-      <c r="E62" s="40"/>
-      <c r="F62" s="40"/>
-      <c r="G62" s="40"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="39"/>
       <c r="H62" s="34"/>
       <c r="I62" s="34"/>
       <c r="J62" s="34"/>
@@ -9854,7 +9843,7 @@
       <c r="M62" s="34"/>
       <c r="N62" s="34"/>
       <c r="T62" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U62" s="2">
@@ -9871,10 +9860,10 @@
       <c r="C63" s="12">
         <v>48</v>
       </c>
-      <c r="D63" s="39"/>
-      <c r="E63" s="39"/>
-      <c r="F63" s="39"/>
-      <c r="G63" s="39"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="40"/>
+      <c r="G63" s="40"/>
       <c r="H63" s="32"/>
       <c r="I63" s="32"/>
       <c r="J63" s="32"/>
@@ -9883,7 +9872,7 @@
       <c r="M63" s="32"/>
       <c r="N63" s="32"/>
       <c r="T63" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U63" s="2">
@@ -9900,10 +9889,10 @@
       <c r="C64" s="13">
         <v>49</v>
       </c>
-      <c r="D64" s="40"/>
-      <c r="E64" s="40"/>
-      <c r="F64" s="40"/>
-      <c r="G64" s="40"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="39"/>
       <c r="H64" s="34"/>
       <c r="I64" s="34"/>
       <c r="J64" s="34"/>
@@ -9912,7 +9901,7 @@
       <c r="M64" s="34"/>
       <c r="N64" s="34"/>
       <c r="T64" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U64" s="2">
@@ -9929,10 +9918,10 @@
       <c r="C65" s="14">
         <v>50</v>
       </c>
-      <c r="D65" s="41"/>
-      <c r="E65" s="41"/>
-      <c r="F65" s="41"/>
-      <c r="G65" s="41"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="45"/>
       <c r="H65" s="36"/>
       <c r="I65" s="36"/>
       <c r="J65" s="36"/>
@@ -9941,7 +9930,7 @@
       <c r="M65" s="36"/>
       <c r="N65" s="36"/>
       <c r="T65" s="1" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U65" s="2">
@@ -10272,46 +10261,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="tjqSiT+XspradLJBNpu0viI4TokIDIF0O7QeXm3BTZLmeAfSOw5TlniSFfStQ9LXJLtK7gLyf3B6jINr+qJ+Cg==" saltValue="/wSmyHkNAfBsPbW8NILu1w==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="56">
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="D39:G39"/>
-    <mergeCell ref="D40:G40"/>
-    <mergeCell ref="D42:G42"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="D50:G50"/>
     <mergeCell ref="D63:G63"/>
     <mergeCell ref="D64:G64"/>
     <mergeCell ref="D65:G65"/>
@@ -10328,6 +10277,46 @@
     <mergeCell ref="D62:G62"/>
     <mergeCell ref="D51:G51"/>
     <mergeCell ref="D52:G52"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="D39:G39"/>
+    <mergeCell ref="D40:G40"/>
+    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="D38:G38"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:N2">
     <cfRule type="expression" dxfId="9" priority="3">
@@ -10452,14 +10441,14 @@
   <sheetData>
     <row r="1" spans="2:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
     </row>
     <row r="3" spans="2:13" ht="10.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>